<commit_message>
hELP LMAO assets(Cuisines and Restaurants.xlsx --> updated the list so no blank space in cuisines) CuisinesListActivity.java res (activity_cuisine_search, all_Cuisines_dislpay_layout)
</commit_message>
<xml_diff>
--- a/app/src/main/Assets/Cuisines and Restaurants.xlsx
+++ b/app/src/main/Assets/Cuisines and Restaurants.xlsx
@@ -1,13 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kel/Documents/GitHub/Orbital_CS_x/app/src/main/Assets/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{280D38D6-6A7F-7847-9D16-F4461FF30085}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Cuisines" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Restaurants" sheetId="2" r:id="rId5"/>
+    <sheet name="Cuisines" sheetId="1" r:id="rId1"/>
+    <sheet name="Restaurants" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -740,50 +749,69 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
       <u/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
+      <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
+      <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="4">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -794,6 +822,8 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -802,6 +832,9 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -810,78 +843,53 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1071,26 +1079,29 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="17.29"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1098,7 +1109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1106,7 +1117,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1114,7 +1125,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1122,7 +1133,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1130,7 +1141,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -1138,7 +1149,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1146,7 +1157,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -1154,7 +1165,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -1162,7 +1173,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1170,361 +1181,362 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="5"/>
-    </row>
-    <row r="12">
+      <c r="C11" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13">
+      <c r="C12" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14">
+      <c r="C13" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15">
+      <c r="C14" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16">
+      <c r="C15" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17">
+      <c r="C16" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18">
+      <c r="C17" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19">
+      <c r="C18" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20">
+      <c r="C19" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21">
+      <c r="C20" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22">
+      <c r="C21" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23">
+      <c r="C22" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24">
+      <c r="C23" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25">
+      <c r="C24" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26">
+      <c r="C25" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="27">
+      <c r="C26" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="28">
+      <c r="C27" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="29">
+      <c r="C28" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
         <v>45</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="31">
+      <c r="C30" s="9"/>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C31" s="9"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C32" s="9"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C33" s="9"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C34" s="9"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C35" s="9"/>
     </row>
-    <row r="36">
+    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C36" s="9"/>
     </row>
-    <row r="37">
+    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C37" s="9"/>
     </row>
-    <row r="38">
+    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="2" t="s">
         <v>50</v>
       </c>
       <c r="C38" s="9"/>
     </row>
-    <row r="39">
+    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C39" s="9"/>
     </row>
-    <row r="40">
+    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="2" t="s">
         <v>52</v>
       </c>
       <c r="C40" s="10"/>
     </row>
-    <row r="41">
+    <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A52" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A53" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A54" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A55" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A56" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A57" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A58" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A59" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A60" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A61" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A62" s="2" t="s">
         <v>47</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1.0" ySplit="1.0" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B1" sqref="B1" pane="topRight"/>
-      <selection activeCell="A2" sqref="A2" pane="bottomLeft"/>
-      <selection activeCell="B2" sqref="B2" pane="bottomRight"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="31.29"/>
-    <col customWidth="1" min="2" max="2" width="18.29"/>
-    <col customWidth="1" min="3" max="3" width="17.29"/>
-    <col customWidth="1" min="4" max="4" width="12.29"/>
+    <col min="1" max="1" width="31.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>67</v>
       </c>
@@ -1550,7 +1562,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>75</v>
       </c>
@@ -1574,7 +1586,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>79</v>
       </c>
@@ -1598,7 +1610,7 @@
       </c>
       <c r="H3" s="14"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>82</v>
       </c>
@@ -1622,7 +1634,7 @@
       </c>
       <c r="H4" s="14"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>85</v>
       </c>
@@ -1644,7 +1656,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>88</v>
       </c>
@@ -1668,7 +1680,7 @@
       </c>
       <c r="H6" s="14"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>91</v>
       </c>
@@ -1692,7 +1704,7 @@
       </c>
       <c r="H7" s="14"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>94</v>
       </c>
@@ -1714,7 +1726,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>97</v>
       </c>
@@ -1738,7 +1750,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>100</v>
       </c>
@@ -1760,7 +1772,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>103</v>
       </c>
@@ -1782,7 +1794,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>106</v>
       </c>
@@ -1804,7 +1816,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>109</v>
       </c>
@@ -1828,7 +1840,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>112</v>
       </c>
@@ -1850,7 +1862,7 @@
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>115</v>
       </c>
@@ -1870,7 +1882,7 @@
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>118</v>
       </c>
@@ -1896,7 +1908,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>121</v>
       </c>
@@ -1918,7 +1930,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>124</v>
       </c>
@@ -1940,7 +1952,7 @@
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>127</v>
       </c>
@@ -1960,7 +1972,7 @@
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>130</v>
       </c>
@@ -1984,7 +1996,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
         <v>133</v>
       </c>
@@ -2008,7 +2020,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="16" t="s">
         <v>136</v>
       </c>
@@ -2026,7 +2038,7 @@
       <c r="G22" s="14"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
         <v>139</v>
       </c>
@@ -2048,7 +2060,7 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
         <v>142</v>
       </c>
@@ -2068,7 +2080,7 @@
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
         <v>145</v>
       </c>
@@ -2094,7 +2106,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
         <v>148</v>
       </c>
@@ -2114,7 +2126,7 @@
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="2" t="s">
         <v>151</v>
       </c>
@@ -2134,7 +2146,7 @@
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="2" t="s">
         <v>154</v>
       </c>
@@ -2156,7 +2168,7 @@
       <c r="G28" s="14"/>
       <c r="H28" s="14"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
         <v>157</v>
       </c>
@@ -2180,7 +2192,7 @@
       </c>
       <c r="H29" s="14"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
         <v>160</v>
       </c>
@@ -2204,7 +2216,7 @@
       </c>
       <c r="H30" s="14"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
         <v>163</v>
       </c>
@@ -2228,7 +2240,7 @@
       </c>
       <c r="H31" s="14"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="2" t="s">
         <v>166</v>
       </c>
@@ -2250,7 +2262,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="2" t="s">
         <v>169</v>
       </c>
@@ -2274,7 +2286,7 @@
       </c>
       <c r="H33" s="14"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="2" t="s">
         <v>172</v>
       </c>
@@ -2298,7 +2310,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="2" t="s">
         <v>175</v>
       </c>
@@ -2324,7 +2336,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="2" t="s">
         <v>178</v>
       </c>
@@ -2348,7 +2360,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="2" t="s">
         <v>181</v>
       </c>
@@ -2374,7 +2386,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="2" t="s">
         <v>184</v>
       </c>
@@ -2396,7 +2408,7 @@
       <c r="G38" s="14"/>
       <c r="H38" s="14"/>
     </row>
-    <row r="39">
+    <row r="39" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="2" t="s">
         <v>187</v>
       </c>
@@ -2418,7 +2430,7 @@
       <c r="G39" s="14"/>
       <c r="H39" s="14"/>
     </row>
-    <row r="40">
+    <row r="40" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="2" t="s">
         <v>190</v>
       </c>
@@ -2440,7 +2452,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="2" t="s">
         <v>193</v>
       </c>
@@ -2464,7 +2476,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="2" t="s">
         <v>196</v>
       </c>
@@ -2488,7 +2500,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="2" t="s">
         <v>199</v>
       </c>
@@ -2512,7 +2524,7 @@
       </c>
       <c r="H43" s="14"/>
     </row>
-    <row r="44">
+    <row r="44" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="2" t="s">
         <v>202</v>
       </c>
@@ -2534,7 +2546,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="2" t="s">
         <v>205</v>
       </c>
@@ -2556,7 +2568,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="2" t="s">
         <v>208</v>
       </c>
@@ -2580,7 +2592,7 @@
       </c>
       <c r="H46" s="14"/>
     </row>
-    <row r="47">
+    <row r="47" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="2" t="s">
         <v>211</v>
       </c>
@@ -2602,7 +2614,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="2" t="s">
         <v>214</v>
       </c>
@@ -2624,7 +2636,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="2" t="s">
         <v>217</v>
       </c>
@@ -2650,7 +2662,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="2" t="s">
         <v>220</v>
       </c>
@@ -2672,7 +2684,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="2" t="s">
         <v>223</v>
       </c>
@@ -2694,7 +2706,7 @@
       <c r="G51" s="14"/>
       <c r="H51" s="14"/>
     </row>
-    <row r="52">
+    <row r="52" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A52" s="2" t="s">
         <v>226</v>
       </c>
@@ -2720,7 +2732,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A53" s="2" t="s">
         <v>229</v>
       </c>
@@ -2744,7 +2756,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A54" s="2" t="s">
         <v>232</v>
       </c>
@@ -2768,7 +2780,7 @@
       </c>
       <c r="H54" s="14"/>
     </row>
-    <row r="55">
+    <row r="55" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A55" s="2" t="s">
         <v>235</v>
       </c>
@@ -2790,7 +2802,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A56" s="2" t="s">
         <v>238</v>
       </c>
@@ -2816,340 +2828,347 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E57" s="14"/>
       <c r="F57" s="14"/>
       <c r="G57" s="14"/>
       <c r="H57" s="14"/>
     </row>
-    <row r="58">
+    <row r="58" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E58" s="14"/>
       <c r="F58" s="14"/>
       <c r="G58" s="14"/>
       <c r="H58" s="14"/>
     </row>
-    <row r="59">
+    <row r="59" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E59" s="14"/>
       <c r="F59" s="14"/>
       <c r="G59" s="14"/>
       <c r="H59" s="14"/>
     </row>
-    <row r="60">
+    <row r="60" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E60" s="14"/>
       <c r="F60" s="14"/>
       <c r="G60" s="14"/>
       <c r="H60" s="14"/>
     </row>
-    <row r="61">
+    <row r="61" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E61" s="14"/>
       <c r="F61" s="14"/>
       <c r="G61" s="14"/>
       <c r="H61" s="14"/>
     </row>
-    <row r="62">
+    <row r="62" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E62" s="14"/>
       <c r="F62" s="14"/>
       <c r="G62" s="14"/>
       <c r="H62" s="14"/>
     </row>
-    <row r="63">
+    <row r="63" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E63" s="14"/>
       <c r="F63" s="14"/>
       <c r="G63" s="14"/>
       <c r="H63" s="14"/>
     </row>
-    <row r="64">
+    <row r="64" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E64" s="14"/>
       <c r="F64" s="14"/>
       <c r="G64" s="14"/>
       <c r="H64" s="14"/>
     </row>
-    <row r="65">
+    <row r="65" spans="5:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E65" s="14"/>
       <c r="F65" s="14"/>
       <c r="G65" s="14"/>
       <c r="H65" s="14"/>
     </row>
-    <row r="66">
+    <row r="66" spans="5:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E66" s="14"/>
       <c r="F66" s="14"/>
       <c r="G66" s="14"/>
       <c r="H66" s="14"/>
     </row>
-    <row r="67">
+    <row r="67" spans="5:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E67" s="14"/>
       <c r="F67" s="14"/>
       <c r="G67" s="14"/>
       <c r="H67" s="14"/>
     </row>
-    <row r="68">
+    <row r="68" spans="5:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E68" s="14"/>
       <c r="F68" s="14"/>
       <c r="G68" s="14"/>
       <c r="H68" s="14"/>
     </row>
-    <row r="69">
+    <row r="69" spans="5:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E69" s="14"/>
       <c r="F69" s="14"/>
       <c r="G69" s="14"/>
       <c r="H69" s="14"/>
     </row>
-    <row r="70">
+    <row r="70" spans="5:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E70" s="14"/>
       <c r="F70" s="14"/>
       <c r="G70" s="14"/>
       <c r="H70" s="14"/>
     </row>
-    <row r="71">
+    <row r="71" spans="5:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E71" s="14"/>
       <c r="F71" s="14"/>
       <c r="G71" s="14"/>
       <c r="H71" s="14"/>
     </row>
-    <row r="72">
+    <row r="72" spans="5:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E72" s="14"/>
       <c r="F72" s="14"/>
       <c r="G72" s="14"/>
       <c r="H72" s="14"/>
     </row>
-    <row r="73">
+    <row r="73" spans="5:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E73" s="14"/>
       <c r="F73" s="14"/>
       <c r="G73" s="14"/>
       <c r="H73" s="14"/>
     </row>
-    <row r="74">
+    <row r="74" spans="5:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E74" s="14"/>
       <c r="F74" s="14"/>
       <c r="G74" s="14"/>
       <c r="H74" s="14"/>
     </row>
-    <row r="75">
+    <row r="75" spans="5:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E75" s="14"/>
       <c r="F75" s="14"/>
       <c r="G75" s="14"/>
       <c r="H75" s="14"/>
     </row>
-    <row r="76">
+    <row r="76" spans="5:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E76" s="14"/>
       <c r="F76" s="14"/>
       <c r="G76" s="14"/>
       <c r="H76" s="14"/>
     </row>
-    <row r="77">
+    <row r="77" spans="5:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E77" s="14"/>
       <c r="F77" s="14"/>
       <c r="G77" s="14"/>
       <c r="H77" s="14"/>
     </row>
-    <row r="78">
+    <row r="78" spans="5:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E78" s="14"/>
       <c r="F78" s="14"/>
       <c r="G78" s="14"/>
       <c r="H78" s="14"/>
     </row>
-    <row r="79">
+    <row r="79" spans="5:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E79" s="14"/>
       <c r="F79" s="14"/>
       <c r="G79" s="14"/>
       <c r="H79" s="14"/>
     </row>
-    <row r="80">
+    <row r="80" spans="5:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E80" s="14"/>
       <c r="F80" s="14"/>
       <c r="G80" s="14"/>
       <c r="H80" s="14"/>
     </row>
-    <row r="81">
+    <row r="81" spans="5:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E81" s="14"/>
       <c r="F81" s="14"/>
       <c r="G81" s="14"/>
       <c r="H81" s="14"/>
     </row>
-    <row r="82">
+    <row r="82" spans="5:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E82" s="14"/>
       <c r="F82" s="14"/>
       <c r="G82" s="14"/>
       <c r="H82" s="14"/>
     </row>
-    <row r="83">
+    <row r="83" spans="5:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E83" s="14"/>
       <c r="F83" s="14"/>
       <c r="G83" s="14"/>
       <c r="H83" s="14"/>
     </row>
-    <row r="84">
+    <row r="84" spans="5:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E84" s="14"/>
       <c r="F84" s="14"/>
       <c r="G84" s="14"/>
       <c r="H84" s="14"/>
     </row>
-    <row r="85">
+    <row r="85" spans="5:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E85" s="14"/>
       <c r="F85" s="14"/>
       <c r="G85" s="14"/>
       <c r="H85" s="14"/>
     </row>
-    <row r="86">
+    <row r="86" spans="5:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E86" s="14"/>
       <c r="F86" s="14"/>
       <c r="G86" s="14"/>
       <c r="H86" s="14"/>
     </row>
-    <row r="87">
+    <row r="87" spans="5:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E87" s="14"/>
       <c r="F87" s="14"/>
       <c r="G87" s="14"/>
       <c r="H87" s="14"/>
     </row>
-    <row r="88">
+    <row r="88" spans="5:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E88" s="14"/>
       <c r="F88" s="14"/>
       <c r="G88" s="14"/>
       <c r="H88" s="14"/>
     </row>
-    <row r="89">
+    <row r="89" spans="5:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E89" s="14"/>
       <c r="F89" s="14"/>
       <c r="G89" s="14"/>
       <c r="H89" s="14"/>
     </row>
-    <row r="90">
+    <row r="90" spans="5:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E90" s="14"/>
       <c r="F90" s="14"/>
       <c r="G90" s="14"/>
       <c r="H90" s="14"/>
     </row>
-    <row r="91">
+    <row r="91" spans="5:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E91" s="14"/>
       <c r="F91" s="14"/>
       <c r="G91" s="14"/>
       <c r="H91" s="14"/>
     </row>
-    <row r="92">
+    <row r="92" spans="5:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E92" s="14"/>
       <c r="F92" s="14"/>
       <c r="G92" s="14"/>
       <c r="H92" s="14"/>
     </row>
-    <row r="93">
+    <row r="93" spans="5:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E93" s="14"/>
       <c r="F93" s="14"/>
       <c r="G93" s="14"/>
       <c r="H93" s="14"/>
     </row>
-    <row r="94">
+    <row r="94" spans="5:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E94" s="14"/>
       <c r="F94" s="14"/>
       <c r="G94" s="14"/>
       <c r="H94" s="14"/>
     </row>
-    <row r="95">
+    <row r="95" spans="5:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E95" s="14"/>
       <c r="F95" s="14"/>
       <c r="G95" s="14"/>
       <c r="H95" s="14"/>
     </row>
-    <row r="96">
+    <row r="96" spans="5:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E96" s="14"/>
       <c r="F96" s="14"/>
       <c r="G96" s="14"/>
       <c r="H96" s="14"/>
     </row>
-    <row r="97">
+    <row r="97" spans="5:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E97" s="14"/>
       <c r="F97" s="14"/>
       <c r="G97" s="14"/>
       <c r="H97" s="14"/>
     </row>
-    <row r="98">
+    <row r="98" spans="5:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E98" s="14"/>
       <c r="F98" s="14"/>
       <c r="G98" s="14"/>
       <c r="H98" s="14"/>
     </row>
-    <row r="99">
+    <row r="99" spans="5:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E99" s="14"/>
       <c r="F99" s="14"/>
       <c r="G99" s="14"/>
       <c r="H99" s="14"/>
     </row>
-    <row r="100">
+    <row r="100" spans="5:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E100" s="14"/>
       <c r="F100" s="14"/>
       <c r="G100" s="14"/>
       <c r="H100" s="14"/>
     </row>
-    <row r="101">
+    <row r="101" spans="5:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E101" s="14"/>
       <c r="F101" s="14"/>
       <c r="G101" s="14"/>
       <c r="H101" s="14"/>
     </row>
   </sheetData>
-  <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="E2:H101">
-      <formula1>Cuisines!$C$2:$C$40</formula1>
-    </dataValidation>
-  </dataValidations>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="A1"/>
-    <hyperlink r:id="rId2" ref="B2"/>
-    <hyperlink r:id="rId3" ref="B3"/>
-    <hyperlink r:id="rId4" ref="B4"/>
-    <hyperlink r:id="rId5" ref="B5"/>
-    <hyperlink r:id="rId6" ref="B6"/>
-    <hyperlink r:id="rId7" ref="B7"/>
-    <hyperlink r:id="rId8" ref="B8"/>
-    <hyperlink r:id="rId9" ref="B9"/>
-    <hyperlink r:id="rId10" ref="B10"/>
-    <hyperlink r:id="rId11" ref="B11"/>
-    <hyperlink r:id="rId12" ref="B12"/>
-    <hyperlink r:id="rId13" ref="B13"/>
-    <hyperlink r:id="rId14" ref="B14"/>
-    <hyperlink r:id="rId15" ref="B15"/>
-    <hyperlink r:id="rId16" ref="B16"/>
-    <hyperlink r:id="rId17" ref="B17"/>
-    <hyperlink r:id="rId18" ref="B18"/>
-    <hyperlink r:id="rId19" ref="B19"/>
-    <hyperlink r:id="rId20" ref="B20"/>
-    <hyperlink r:id="rId21" ref="B21"/>
-    <hyperlink r:id="rId22" ref="B22"/>
-    <hyperlink r:id="rId23" ref="B23"/>
-    <hyperlink r:id="rId24" ref="B24"/>
-    <hyperlink r:id="rId25" ref="B25"/>
-    <hyperlink r:id="rId26" ref="B26"/>
-    <hyperlink r:id="rId27" ref="B27"/>
-    <hyperlink r:id="rId28" ref="B28"/>
-    <hyperlink r:id="rId29" ref="B29"/>
-    <hyperlink r:id="rId30" ref="B30"/>
-    <hyperlink r:id="rId31" ref="B31"/>
-    <hyperlink r:id="rId32" ref="B32"/>
-    <hyperlink r:id="rId33" ref="B33"/>
-    <hyperlink r:id="rId34" ref="B34"/>
-    <hyperlink r:id="rId35" ref="B35"/>
-    <hyperlink r:id="rId36" ref="B36"/>
-    <hyperlink r:id="rId37" ref="B37"/>
-    <hyperlink r:id="rId38" ref="B38"/>
-    <hyperlink r:id="rId39" ref="B39"/>
-    <hyperlink r:id="rId40" ref="B40"/>
-    <hyperlink r:id="rId41" ref="B41"/>
-    <hyperlink r:id="rId42" ref="B42"/>
-    <hyperlink r:id="rId43" ref="B43"/>
-    <hyperlink r:id="rId44" ref="B44"/>
-    <hyperlink r:id="rId45" ref="B45"/>
-    <hyperlink r:id="rId46" ref="B46"/>
-    <hyperlink r:id="rId47" ref="B47"/>
-    <hyperlink r:id="rId48" ref="B48"/>
-    <hyperlink r:id="rId49" ref="B49"/>
-    <hyperlink r:id="rId50" ref="B50"/>
-    <hyperlink r:id="rId51" ref="B51"/>
-    <hyperlink r:id="rId52" ref="B52"/>
-    <hyperlink r:id="rId53" ref="B53"/>
-    <hyperlink r:id="rId54" ref="B54"/>
-    <hyperlink r:id="rId55" ref="B55"/>
-    <hyperlink r:id="rId56" ref="B56"/>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="B5" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="B6" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="B7" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="B8" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="B9" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="B10" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="B11" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="B12" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="B13" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="B14" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="B15" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="B16" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="B17" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="B18" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="B19" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
+    <hyperlink ref="B20" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
+    <hyperlink ref="B21" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="B22" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
+    <hyperlink ref="B23" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
+    <hyperlink ref="B24" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
+    <hyperlink ref="B25" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink ref="B26" r:id="rId26" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
+    <hyperlink ref="B27" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
+    <hyperlink ref="B28" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
+    <hyperlink ref="B29" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink ref="B30" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
+    <hyperlink ref="B31" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink ref="B32" r:id="rId32" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
+    <hyperlink ref="B33" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
+    <hyperlink ref="B34" r:id="rId34" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
+    <hyperlink ref="B35" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
+    <hyperlink ref="B36" r:id="rId36" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
+    <hyperlink ref="B37" r:id="rId37" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
+    <hyperlink ref="B38" r:id="rId38" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
+    <hyperlink ref="B39" r:id="rId39" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
+    <hyperlink ref="B40" r:id="rId40" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
+    <hyperlink ref="B41" r:id="rId41" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
+    <hyperlink ref="B42" r:id="rId42" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
+    <hyperlink ref="B43" r:id="rId43" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
+    <hyperlink ref="B44" r:id="rId44" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
+    <hyperlink ref="B45" r:id="rId45" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
+    <hyperlink ref="B46" r:id="rId46" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
+    <hyperlink ref="B47" r:id="rId47" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
+    <hyperlink ref="B48" r:id="rId48" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
+    <hyperlink ref="B49" r:id="rId49" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
+    <hyperlink ref="B50" r:id="rId50" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
+    <hyperlink ref="B51" r:id="rId51" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
+    <hyperlink ref="B52" r:id="rId52" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
+    <hyperlink ref="B53" r:id="rId53" xr:uid="{00000000-0004-0000-0100-000034000000}"/>
+    <hyperlink ref="B54" r:id="rId54" xr:uid="{00000000-0004-0000-0100-000035000000}"/>
+    <hyperlink ref="B55" r:id="rId55" xr:uid="{00000000-0004-0000-0100-000036000000}"/>
+    <hyperlink ref="B56" r:id="rId56" xr:uid="{00000000-0004-0000-0100-000037000000}"/>
   </hyperlinks>
-  <drawing r:id="rId57"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
+          <x14:formula1>
+            <xm:f>Cuisines!$C$2:$C$40</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:H101</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>